<commit_message>
updates voltages for ifcb1 with new laser
</commit_message>
<xml_diff>
--- a/IFCB_tools/IFCB_beadvoltages_temp.xlsx
+++ b/IFCB_tools/IFCB_beadvoltages_temp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IFCB10" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="167">
   <si>
     <t>File D</t>
   </si>
@@ -506,6 +506,36 @@
   </si>
   <si>
     <t>9um beads in SW after changing delay to about 270us guess that's not what it was before. Could be new board?</t>
+  </si>
+  <si>
+    <t>4.5-5V</t>
+  </si>
+  <si>
+    <t>chl hv</t>
+  </si>
+  <si>
+    <t>new laser after lightening strike</t>
+  </si>
+  <si>
+    <t>IFCB1_036_165039</t>
+  </si>
+  <si>
+    <t>0.3-0.6</t>
+  </si>
+  <si>
+    <t>2.5-3.2</t>
+  </si>
+  <si>
+    <t>IFCB1_036_172753</t>
+  </si>
+  <si>
+    <t>2.5-3.1</t>
+  </si>
+  <si>
+    <t>use all signals, realign who camera/PMT stack,pump1</t>
+  </si>
+  <si>
+    <t>use all signals, realign who camera/PMT stack,pump2</t>
   </si>
 </sst>
 </file>
@@ -1342,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,20 +1383,20 @@
     <col min="1" max="1" width="26" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="2"/>
-    <col min="16" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="2"/>
+    <col min="17" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1379,38 +1409,41 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -1423,41 +1456,41 @@
       <c r="D2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>2</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>6.5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>19.2</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>0.35</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>6.5</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>19.2</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
@@ -1470,38 +1503,38 @@
       <c r="D3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>7.2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>9.5</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>0.38</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>18.8</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>33.4</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -1514,38 +1547,38 @@
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>10.9</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>25.6</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0.61</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>40.9</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>45.1</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -1558,38 +1591,38 @@
       <c r="D5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>9</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>0.62</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>41.2</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>30</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
@@ -1602,38 +1635,38 @@
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>10.199999999999999</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>27.4</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>0.61</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>41.3</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>47.5</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1646,44 +1679,44 @@
       <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>11.1</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>27.5</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>43.8</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>43.5</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -1696,44 +1729,44 @@
       <c r="D8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>2.1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>8.6</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>22.4</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>0.32</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>14.8</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>35</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>66</v>
       </c>
@@ -1746,41 +1779,41 @@
       <c r="D9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>7.9</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>20.9</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>0.27</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>35.5</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>62.9</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
@@ -1793,35 +1826,35 @@
       <c r="D10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>8.5</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>14.9</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>0.32</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>42.5</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>59.1</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -1834,29 +1867,29 @@
       <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>10.199999999999999</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>30.1</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>0.35</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>29.6</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>76.3</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
@@ -1869,29 +1902,29 @@
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>11</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>29.9</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>0.33</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>41.9</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>105.4</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>145</v>
       </c>
@@ -1904,38 +1937,137 @@
       <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>2</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>8.6</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>13.4</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>0.3</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>27.7</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>63.2</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>42389</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="6">
+        <v>42405</v>
+      </c>
+      <c r="C15" s="3">
+        <v>165039</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="H15" s="3">
+        <v>29.8</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="K15" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L15" s="3">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="6">
+        <v>42405</v>
+      </c>
+      <c r="C16" s="3">
+        <v>172753</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="H16" s="3">
+        <v>26.9</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="K16" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="L16" s="3">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1948,7 +2080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated ifcb10 laser alignment signals
</commit_message>
<xml_diff>
--- a/IFCB_tools/IFCB_beadvoltages_temp.xlsx
+++ b/IFCB_tools/IFCB_beadvoltages_temp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290"/>
   </bookViews>
   <sheets>
     <sheet name="IFCB10" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="177">
   <si>
     <t>File D</t>
   </si>
@@ -536,6 +536,38 @@
   </si>
   <si>
     <t>use all signals, realign who camera/PMT stack,pump2</t>
+  </si>
+  <si>
+    <t>PMTA
+calc peak</t>
+  </si>
+  <si>
+    <t>PMTA
+calc int</t>
+  </si>
+  <si>
+    <t>1.2-1.6</t>
+  </si>
+  <si>
+    <t>0.1-0.2</t>
+  </si>
+  <si>
+    <t>NAN</t>
+  </si>
+  <si>
+    <t>completely realigned laser including move PMTS because camera at edge of adjustment and delay at 10us, move laser down when looking at telescope</t>
+  </si>
+  <si>
+    <t>pump1 us all signals</t>
+  </si>
+  <si>
+    <t>0.8-1.15</t>
+  </si>
+  <si>
+    <t>selected points single beads</t>
+  </si>
+  <si>
+    <t>adjusted laser vert,horz,foc again after moving needle and then camera stack</t>
   </si>
 </sst>
 </file>
@@ -907,19 +939,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -927,442 +960,551 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20141209</v>
       </c>
       <c r="B2">
         <v>204349</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.67591999999999997</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>6.2895999999999994E-2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>0.22331999999999999</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>0.10234</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>0.14701</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20141210</v>
       </c>
       <c r="B3">
         <v>212839</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.58399999999999996</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>5.1700000000000003E-2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>0.25579000000000002</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>0.10033</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>0.26891999999999999</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>0.24443999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20141230</v>
       </c>
       <c r="B4">
         <v>150002</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.61348999999999998</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5.3900000000000003E-2</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.06</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>0.23027</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>0.10524</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>0.28575</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>0.1242</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20141230</v>
       </c>
       <c r="B5">
         <v>171010</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.5</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.36105999999999999</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>4.0980000000000003E-2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>0.24640000000000001</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>0.12293</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>0.18845000000000001</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>0.1067</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20141230</v>
       </c>
       <c r="B6">
         <v>201059</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.36103000000000002</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3.9972000000000001E-2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>0.24060000000000001</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>0.10503</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>0.26929999999999998</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>0.1164</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20141231</v>
       </c>
       <c r="B7">
         <v>201115</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.65878000000000003</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>6.3239000000000004E-2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>0.24712999999999999</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>9.1675000000000006E-2</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>0.21318000000000001</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>0.11756</v>
       </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
         <v>19</v>
       </c>
-      <c r="M7" t="s">
+      <c r="P7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20141231</v>
       </c>
       <c r="B8">
         <v>204115</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.65732000000000002</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>6.2505000000000005E-2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>0.21526999999999999</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>9.4182000000000002E-2</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>0.23630000000000001</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>0.11747</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20150102</v>
       </c>
       <c r="B9">
         <v>160459</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.61556999999999995</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>6.3796000000000005E-2</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.06</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>26</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>0.28088000000000002</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>27</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>0.26277</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>0.17221</v>
       </c>
-      <c r="L9" t="s">
+      <c r="O9" t="s">
         <v>24</v>
       </c>
-      <c r="M9" t="s">
+      <c r="P9" t="s">
         <v>25</v>
       </c>
-      <c r="N9" t="s">
+      <c r="Q9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20150102</v>
       </c>
       <c r="B10">
         <v>162205</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.60019999999999996</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>6.2342000000000002E-2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>0.22997000000000001</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>9.3048000000000006E-2</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>0.24102000000000001</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>0.14566000000000001</v>
       </c>
-      <c r="L10" t="s">
+      <c r="O10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="L11" t="s">
+      <c r="O11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20150116</v>
       </c>
       <c r="B12">
         <v>160920</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.56521999999999994</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>82</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>83</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>0.17365</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>0.17927000000000001</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>0.24102999999999999</v>
       </c>
-      <c r="L12" t="s">
+      <c r="O12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20150116</v>
       </c>
       <c r="B13">
         <v>163330</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>88</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.61004000000000003</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>5.5225000000000003E-2</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>85</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>86</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>0.16611000000000001</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>0.18115000000000001</v>
       </c>
-      <c r="J13">
+      <c r="M13">
         <v>0.25202000000000002</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>0.11573</v>
       </c>
-      <c r="L13" t="s">
+      <c r="O13" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20160321</v>
+      </c>
+      <c r="B14">
+        <v>201207</v>
+      </c>
+      <c r="C14">
+        <v>0.7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>1.3754</v>
+      </c>
+      <c r="F14">
+        <v>0.1227</v>
+      </c>
+      <c r="G14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14">
+        <v>3.4763000000000002</v>
+      </c>
+      <c r="J14">
+        <v>0.30814000000000002</v>
+      </c>
+      <c r="K14" t="s">
+        <v>171</v>
+      </c>
+      <c r="L14" t="s">
+        <v>171</v>
+      </c>
+      <c r="M14" t="s">
+        <v>171</v>
+      </c>
+      <c r="N14">
+        <v>0.11645</v>
+      </c>
+      <c r="O14" t="s">
+        <v>172</v>
+      </c>
+      <c r="P14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20160323</v>
+      </c>
+      <c r="B15">
+        <v>212722</v>
+      </c>
+      <c r="C15">
+        <v>0.7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>0.93152999999999997</v>
+      </c>
+      <c r="F15">
+        <v>0.10829</v>
+      </c>
+      <c r="G15" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" t="s">
+        <v>174</v>
+      </c>
+      <c r="I15">
+        <v>2.9788999999999999</v>
+      </c>
+      <c r="J15">
+        <v>0.28516000000000002</v>
+      </c>
+      <c r="K15">
+        <v>0.20415</v>
+      </c>
+      <c r="L15">
+        <v>0.10391</v>
+      </c>
+      <c r="M15">
+        <v>0.25572</v>
+      </c>
+      <c r="N15">
+        <v>8.6920999999999998E-2</v>
+      </c>
+      <c r="O15" t="s">
+        <v>175</v>
+      </c>
+      <c r="P15" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add ifcb109 to list
</commit_message>
<xml_diff>
--- a/IFCB_tools/IFCB_beadvoltages_temp.xlsx
+++ b/IFCB_tools/IFCB_beadvoltages_temp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IFCB10" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="IFCB5" sheetId="3" r:id="rId3"/>
     <sheet name="IFCB101" sheetId="4" r:id="rId4"/>
     <sheet name="IFCB102" sheetId="5" r:id="rId5"/>
+    <sheet name="IFCB109" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="198">
   <si>
     <t>File D</t>
   </si>
@@ -568,6 +569,70 @@
   </si>
   <si>
     <t>adjusted laser vert,horz,foc again after moving needle and then camera stack</t>
+  </si>
+  <si>
+    <t>did not move laser for previous file but slightly moved nuts securing camera stack</t>
+  </si>
+  <si>
+    <t>0.1-0.17</t>
+  </si>
+  <si>
+    <t>1-1.6</t>
+  </si>
+  <si>
+    <t>IFCB5_2016_085_151306</t>
+  </si>
+  <si>
+    <t>ChA 
+CV(half-Int)</t>
+  </si>
+  <si>
+    <t>IFCB5_2016_088_174108</t>
+  </si>
+  <si>
+    <t>1.3-2.2</t>
+  </si>
+  <si>
+    <t>select single bead signals, file after recovery due to bad flow, 9um beads in FSW</t>
+  </si>
+  <si>
+    <t>select single beads, post micro/Q cleaning, 9um beads in FSW</t>
+  </si>
+  <si>
+    <t>1.5-2</t>
+  </si>
+  <si>
+    <t>pump1</t>
+  </si>
+  <si>
+    <t>IFCB5_2016_153_210249</t>
+  </si>
+  <si>
+    <t>1.2-1.7</t>
+  </si>
+  <si>
+    <t>0.5-1.3</t>
+  </si>
+  <si>
+    <t>use all signals, old mildly dirty beads, somewhat out of focus</t>
+  </si>
+  <si>
+    <t>after 2week test weel, 1 month sit in hallway, not good flow so soak micro 40min, then looks good</t>
+  </si>
+  <si>
+    <t>pump2</t>
+  </si>
+  <si>
+    <t>hvA</t>
+  </si>
+  <si>
+    <t>0.03-0.06</t>
+  </si>
+  <si>
+    <t>PMTvoltages low</t>
+  </si>
+  <si>
+    <t>fresh 9um beads in FSW</t>
   </si>
 </sst>
 </file>
@@ -633,8 +698,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,6 +1570,56 @@
       </c>
       <c r="P15" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20160324</v>
+      </c>
+      <c r="B16">
+        <v>170421</v>
+      </c>
+      <c r="C16">
+        <v>0.7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>1.3308</v>
+      </c>
+      <c r="F16">
+        <v>0.14124</v>
+      </c>
+      <c r="G16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" t="s">
+        <v>179</v>
+      </c>
+      <c r="I16">
+        <v>3.1798999999999999</v>
+      </c>
+      <c r="J16">
+        <v>0.14124</v>
+      </c>
+      <c r="K16">
+        <v>0.20268</v>
+      </c>
+      <c r="L16">
+        <v>0.10203</v>
+      </c>
+      <c r="M16">
+        <v>0.20662</v>
+      </c>
+      <c r="N16">
+        <v>0.10088999999999999</v>
+      </c>
+      <c r="O16" t="s">
+        <v>175</v>
+      </c>
+      <c r="P16" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2220,17 +2335,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="10" customWidth="1"/>
     <col min="8" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
@@ -2253,7 +2368,7 @@
         <v>54</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>55</v>
+        <v>181</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>56</v>
@@ -2288,8 +2403,8 @@
       <c r="B2" s="8">
         <v>42033</v>
       </c>
-      <c r="C2" s="9">
-        <v>0.95000000000000007</v>
+      <c r="C2" s="10">
+        <v>2248</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -2329,8 +2444,8 @@
       <c r="B3" s="8">
         <v>42289</v>
       </c>
-      <c r="C3" s="9">
-        <v>0.42152777777777778</v>
+      <c r="C3" s="10">
+        <v>1007</v>
       </c>
       <c r="E3">
         <v>1.6</v>
@@ -2354,8 +2469,135 @@
         <v>156</v>
       </c>
     </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="8">
+        <v>42454</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1513</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>1.7</v>
+      </c>
+      <c r="F4">
+        <v>9.6</v>
+      </c>
+      <c r="G4">
+        <v>8.1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>186</v>
+      </c>
+      <c r="I4">
+        <v>0.88</v>
+      </c>
+      <c r="J4">
+        <v>25.9</v>
+      </c>
+      <c r="K4">
+        <v>21.7</v>
+      </c>
+      <c r="M4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="8">
+        <v>42457</v>
+      </c>
+      <c r="C5" s="10">
+        <v>174108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>1.6</v>
+      </c>
+      <c r="F5">
+        <v>14.9</v>
+      </c>
+      <c r="G5">
+        <v>12.2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I5">
+        <v>0.92</v>
+      </c>
+      <c r="J5">
+        <v>23.3</v>
+      </c>
+      <c r="K5">
+        <v>18.3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>185</v>
+      </c>
+      <c r="N5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="8">
+        <v>42523</v>
+      </c>
+      <c r="C6" s="10">
+        <v>210249</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>1.4</v>
+      </c>
+      <c r="F6">
+        <v>7.3</v>
+      </c>
+      <c r="G6">
+        <v>38.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>189</v>
+      </c>
+      <c r="I6">
+        <v>0.67</v>
+      </c>
+      <c r="J6">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="K6">
+        <v>49.2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>190</v>
+      </c>
+      <c r="M6" t="s">
+        <v>191</v>
+      </c>
+      <c r="N6" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2419,7 +2661,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>20150204</v>
       </c>
       <c r="B2">
@@ -2463,7 +2705,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>20150204</v>
       </c>
       <c r="B3">
@@ -2551,7 +2793,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>20150210</v>
       </c>
       <c r="B5">
@@ -2589,7 +2831,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>20150210</v>
       </c>
       <c r="B6">
@@ -2630,7 +2872,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>20150210</v>
       </c>
       <c r="B7">
@@ -2668,7 +2910,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>20150210</v>
       </c>
       <c r="B8">
@@ -2709,7 +2951,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>20150212</v>
       </c>
       <c r="B9">
@@ -2812,7 +3054,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>20141104</v>
       </c>
       <c r="B2">
@@ -2850,7 +3092,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>20150223</v>
       </c>
       <c r="B3">
@@ -2926,7 +3168,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>20140302</v>
       </c>
       <c r="B5">
@@ -2958,7 +3200,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>20150313</v>
       </c>
       <c r="B6">
@@ -3005,7 +3247,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>20150316</v>
       </c>
       <c r="B7">
@@ -3055,7 +3297,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>20150616</v>
       </c>
       <c r="B8">
@@ -3096,7 +3338,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>20150616</v>
       </c>
       <c r="B9">
@@ -3132,6 +3374,157 @@
       <c r="M9" t="s">
         <v>150</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>20160512</v>
+      </c>
+      <c r="B2">
+        <v>193524</v>
+      </c>
+      <c r="C2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>0.60899000000000003</v>
+      </c>
+      <c r="F2">
+        <v>4.3404999999999999E-2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2">
+        <v>0.45</v>
+      </c>
+      <c r="J2">
+        <v>0.54779999999999995</v>
+      </c>
+      <c r="K2">
+        <v>3.1928999999999999E-2</v>
+      </c>
+      <c r="L2">
+        <v>0.31685000000000002</v>
+      </c>
+      <c r="M2">
+        <v>0.10389</v>
+      </c>
+      <c r="N2">
+        <v>0.24601999999999999</v>
+      </c>
+      <c r="O2">
+        <v>9.5977000000000007E-2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="Q7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ifcb109 laser alignmen files
</commit_message>
<xml_diff>
--- a/IFCB_tools/IFCB_beadvoltages_temp.xlsx
+++ b/IFCB_tools/IFCB_beadvoltages_temp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="206">
   <si>
     <t>File D</t>
   </si>
@@ -633,6 +633,30 @@
   </si>
   <si>
     <t>fresh 9um beads in FSW</t>
+  </si>
+  <si>
+    <t>very skewed</t>
+  </si>
+  <si>
+    <t>1.0-2.0</t>
+  </si>
+  <si>
+    <t>0.05-0.15</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>moving laser a lot, is this acceptable alignment?</t>
+  </si>
+  <si>
+    <t>select out singlet beads, a few 20um and doublets in there</t>
+  </si>
+  <si>
+    <t>0.75-1.15</t>
+  </si>
+  <si>
+    <t>0.045-0.07</t>
   </si>
 </sst>
 </file>
@@ -674,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,6 +724,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3386,7 +3411,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3506,7 +3531,95 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="9">
+        <v>20160718</v>
+      </c>
+      <c r="B3">
+        <v>213034</v>
+      </c>
+      <c r="C3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>1.3986000000000001</v>
+      </c>
+      <c r="F3">
+        <v>7.7092999999999995E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="I3">
+        <v>0.5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K3" t="s">
+        <v>201</v>
+      </c>
+      <c r="P3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20160721</v>
+      </c>
+      <c r="B4">
+        <v>155707</v>
+      </c>
+      <c r="C4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="F4">
+        <v>5.8625999999999998E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H4" t="s">
+        <v>204</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+      <c r="J4">
+        <v>1.5671999999999999</v>
+      </c>
+      <c r="K4">
+        <v>9.0564000000000006E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.24626000000000001</v>
+      </c>
+      <c r="M4">
+        <v>0.11241</v>
+      </c>
+      <c r="N4">
+        <v>0.18114</v>
+      </c>
+      <c r="O4">
+        <v>0.10228</v>
+      </c>
+      <c r="P4" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>

</xml_diff>

<commit_message>
internal beads hvb 0.62
</commit_message>
<xml_diff>
--- a/IFCB_tools/IFCB_beadvoltages_temp.xlsx
+++ b/IFCB_tools/IFCB_beadvoltages_temp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IFCB10" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="208">
   <si>
     <t>File D</t>
   </si>
@@ -657,6 +657,12 @@
   </si>
   <si>
     <t>0.045-0.07</t>
+  </si>
+  <si>
+    <t>1.5-3.5</t>
+  </si>
+  <si>
+    <t>internal beads use all signals</t>
   </si>
 </sst>
 </file>
@@ -3410,8 +3416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3622,7 +3628,51 @@
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="9">
+        <v>20160723</v>
+      </c>
+      <c r="B5">
+        <v>140329</v>
+      </c>
+      <c r="C5">
+        <v>0.62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5">
+        <v>2.4339</v>
+      </c>
+      <c r="F5">
+        <v>0.16642999999999999</v>
+      </c>
+      <c r="G5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5">
+        <v>0.5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K5">
+        <v>8.1054000000000001E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.27424999999999999</v>
+      </c>
+      <c r="M5">
+        <v>0.15379999999999999</v>
+      </c>
+      <c r="N5">
+        <v>0.24159</v>
+      </c>
+      <c r="P5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>

</xml_diff>